<commit_message>
made a pretty graph for exp2
</commit_message>
<xml_diff>
--- a/lab4/2/exp2.xlsx
+++ b/lab4/2/exp2.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="exp2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -3279,11 +3279,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75871296"/>
-        <c:axId val="75870720"/>
+        <c:axId val="43031296"/>
+        <c:axId val="43031872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75871296"/>
+        <c:axId val="43031296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3297,12 +3297,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75870720"/>
+        <c:crossAx val="43031872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75870720"/>
+        <c:axId val="43031872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3317,7 +3317,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75871296"/>
+        <c:crossAx val="43031296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>